<commit_message>
Updated DUI traffic data, comlpeted V1.3 documentation, added static EDA script for the court cases
</commit_message>
<xml_diff>
--- a/dashboard_data/dashboard_data_v_1_3_METADATA.xlsx
+++ b/dashboard_data/dashboard_data_v_1_3_METADATA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\met48\Desktop\V1.3_CHERR-mental_health_data_processing\dashboard_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1718C2C-3B97-4B26-BAB2-9E777674A914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ABA0E8A-A132-4324-849A-F5557E1C1743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="405" yWindow="255" windowWidth="24630" windowHeight="14175" xr2:uid="{39900F9C-C46F-4183-957F-FA1EA2F9375C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{39900F9C-C46F-4183-957F-FA1EA2F9375C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -799,8 +799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07A3EC8F-C693-455A-9BCD-06F94A57406A}">
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1060,7 +1060,9 @@
       <c r="D15" t="s">
         <v>81</v>
       </c>
-      <c r="E15" s="1"/>
+      <c r="E15" s="1">
+        <v>2020</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1791,7 +1793,9 @@
       <c r="D59" t="s">
         <v>112</v>
       </c>
-      <c r="E59" s="1"/>
+      <c r="E59" s="1">
+        <v>2019</v>
+      </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
@@ -1806,7 +1810,9 @@
       <c r="D60" t="s">
         <v>113</v>
       </c>
-      <c r="E60" s="1"/>
+      <c r="E60" s="1">
+        <v>2019</v>
+      </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
@@ -1821,7 +1827,9 @@
       <c r="D61" t="s">
         <v>114</v>
       </c>
-      <c r="E61" s="1"/>
+      <c r="E61" s="1">
+        <v>2019</v>
+      </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
@@ -1836,7 +1844,9 @@
       <c r="D62" t="s">
         <v>115</v>
       </c>
-      <c r="E62" s="1"/>
+      <c r="E62" s="1">
+        <v>2019</v>
+      </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">

</xml_diff>